<commit_message>
assignment week 7,8 + Update new version DB
</commit_message>
<xml_diff>
--- a/Assigment.xlsx
+++ b/Assigment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,60 @@
   </si>
   <si>
     <t>deadline thứ 6 19/4/2019</t>
+  </si>
+  <si>
+    <t>Tuần 6:</t>
+  </si>
+  <si>
+    <t>1. Chức năng đăng tin (video) để promotion về địa điểm du lịch của Tour Guide</t>
+  </si>
+  <si>
+    <t>2. Quản lý tin đăng (Tour Guide) (Manage seft tour)</t>
+  </si>
+  <si>
+    <t>Tuần 7 :</t>
+  </si>
+  <si>
+    <t>1. Chức năng View Tour + Search Tour.</t>
+  </si>
+  <si>
+    <t>2. Chức năng Chat</t>
+  </si>
+  <si>
+    <t>3. Chức năng Book Tour</t>
+  </si>
+  <si>
+    <t>4. Chức năng FeedBack</t>
+  </si>
+  <si>
+    <t>Tuần 6</t>
+  </si>
+  <si>
+    <t>Tuần 7</t>
+  </si>
+  <si>
+    <t>Tuần 8 :</t>
+  </si>
+  <si>
+    <t>1. QL User</t>
+  </si>
+  <si>
+    <t>2. QL Tour</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Quản lý tin đăng (Tour Guide) (Manage seft tour).
+</t>
+  </si>
+  <si>
+    <t>1. Chức năng View Tour + Search Tour.
+4. Chức năng FeedBack.</t>
+  </si>
+  <si>
+    <t>2. Chức năng Chat.
+3. Chức năng Book Tour.</t>
   </si>
 </sst>
 </file>
@@ -131,12 +185,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -144,21 +198,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F6"/>
+  <dimension ref="A3:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -477,9 +623,11 @@
     <col min="4" max="4" width="18.25" customWidth="1"/>
     <col min="5" max="5" width="23.375" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,12 +646,18 @@
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -518,12 +672,18 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -536,8 +696,14 @@
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -547,8 +713,82 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="13" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>